<commit_message>
helpers for issue and declared sum
</commit_message>
<xml_diff>
--- a/files/test.xlsx
+++ b/files/test.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AX4"/>
+  <dimension ref="A1:AX2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -556,22 +556,22 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>20230809</v>
+        <v>20230810</v>
       </c>
       <c r="B2" t="str">
-        <v>861690556803</v>
+        <v>951690564664</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>1559</v>
       </c>
       <c r="D2">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="E2">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="F2" t="str">
-        <v>20230809</v>
+        <v>20230810</v>
       </c>
       <c r="G2" t="str">
         <v/>
@@ -583,16 +583,16 @@
         <v>1</v>
       </c>
       <c r="J2" t="str">
-        <v>04361</v>
+        <v>19749</v>
       </c>
       <c r="K2" t="str">
         <v>010</v>
       </c>
       <c r="L2" t="str">
-        <v>Вострикова Татьяна Анатольевна</v>
+        <v>Абубякяров Ильдус</v>
       </c>
       <c r="M2" t="str">
-        <v>79859956612</v>
+        <v>79299431323</v>
       </c>
       <c r="N2" t="str">
         <v/>
@@ -702,317 +702,13 @@
       <c r="AW2" t="str">
         <v/>
       </c>
-      <c r="AX2" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>20230809</v>
-      </c>
-      <c r="B3" t="str">
-        <v>911690694243</v>
-      </c>
-      <c r="C3">
-        <v>10125</v>
-      </c>
-      <c r="D3">
-        <v>350</v>
-      </c>
-      <c r="E3">
-        <v>350</v>
-      </c>
-      <c r="F3" t="str">
-        <v>20230809</v>
-      </c>
-      <c r="G3" t="str">
-        <v/>
-      </c>
-      <c r="H3" t="str">
-        <v/>
-      </c>
-      <c r="I3" t="str">
+      <c r="AX2">
         <v>1</v>
-      </c>
-      <c r="J3" t="str">
-        <v>04216</v>
-      </c>
-      <c r="K3" t="str">
-        <v>010</v>
-      </c>
-      <c r="L3" t="str">
-        <v>Дырина Анастасия  Михайловна</v>
-      </c>
-      <c r="M3" t="str">
-        <v>79270918918</v>
-      </c>
-      <c r="N3" t="str">
-        <v/>
-      </c>
-      <c r="O3" t="str">
-        <v/>
-      </c>
-      <c r="P3" t="str">
-        <v/>
-      </c>
-      <c r="Q3" t="str">
-        <v/>
-      </c>
-      <c r="R3" t="str">
-        <v/>
-      </c>
-      <c r="S3" t="str">
-        <v/>
-      </c>
-      <c r="T3" t="str">
-        <v/>
-      </c>
-      <c r="U3" t="str">
-        <v/>
-      </c>
-      <c r="V3" t="str">
-        <v/>
-      </c>
-      <c r="W3" t="str">
-        <v/>
-      </c>
-      <c r="X3" t="str">
-        <v>3000</v>
-      </c>
-      <c r="Y3" t="str">
-        <v/>
-      </c>
-      <c r="Z3" t="str">
-        <v/>
-      </c>
-      <c r="AA3" t="str">
-        <v/>
-      </c>
-      <c r="AB3" t="str">
-        <v/>
-      </c>
-      <c r="AC3" t="str">
-        <v/>
-      </c>
-      <c r="AD3" t="str">
-        <v/>
-      </c>
-      <c r="AE3" t="str">
-        <v/>
-      </c>
-      <c r="AF3" t="str">
-        <v/>
-      </c>
-      <c r="AG3" t="str">
-        <v/>
-      </c>
-      <c r="AH3" t="str">
-        <v/>
-      </c>
-      <c r="AI3" t="str">
-        <v/>
-      </c>
-      <c r="AJ3" t="str">
-        <v/>
-      </c>
-      <c r="AK3" t="str">
-        <v/>
-      </c>
-      <c r="AL3" t="str">
-        <v/>
-      </c>
-      <c r="AM3" t="str">
-        <v/>
-      </c>
-      <c r="AN3" t="str">
-        <v/>
-      </c>
-      <c r="AO3" t="str">
-        <v/>
-      </c>
-      <c r="AP3" t="str">
-        <v/>
-      </c>
-      <c r="AQ3" t="str">
-        <v/>
-      </c>
-      <c r="AR3" t="str">
-        <v/>
-      </c>
-      <c r="AS3" t="str">
-        <v/>
-      </c>
-      <c r="AT3" t="str">
-        <v/>
-      </c>
-      <c r="AU3" t="str">
-        <v/>
-      </c>
-      <c r="AV3" t="str">
-        <v/>
-      </c>
-      <c r="AW3" t="str">
-        <v/>
-      </c>
-      <c r="AX3" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>20230809</v>
-      </c>
-      <c r="B4" t="str">
-        <v>761690553489</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>250</v>
-      </c>
-      <c r="E4">
-        <v>250</v>
-      </c>
-      <c r="F4" t="str">
-        <v>20230809</v>
-      </c>
-      <c r="G4" t="str">
-        <v/>
-      </c>
-      <c r="H4" t="str">
-        <v/>
-      </c>
-      <c r="I4" t="str">
-        <v>1</v>
-      </c>
-      <c r="J4" t="str">
-        <v>17731</v>
-      </c>
-      <c r="K4" t="str">
-        <v>010</v>
-      </c>
-      <c r="L4" t="str">
-        <v>Ефремова  Юлия Владимировна</v>
-      </c>
-      <c r="M4" t="str">
-        <v>79162207953</v>
-      </c>
-      <c r="N4" t="str">
-        <v/>
-      </c>
-      <c r="O4" t="str">
-        <v/>
-      </c>
-      <c r="P4" t="str">
-        <v/>
-      </c>
-      <c r="Q4" t="str">
-        <v/>
-      </c>
-      <c r="R4" t="str">
-        <v/>
-      </c>
-      <c r="S4" t="str">
-        <v/>
-      </c>
-      <c r="T4" t="str">
-        <v/>
-      </c>
-      <c r="U4" t="str">
-        <v/>
-      </c>
-      <c r="V4" t="str">
-        <v/>
-      </c>
-      <c r="W4" t="str">
-        <v/>
-      </c>
-      <c r="X4" t="str">
-        <v>3000</v>
-      </c>
-      <c r="Y4" t="str">
-        <v/>
-      </c>
-      <c r="Z4" t="str">
-        <v/>
-      </c>
-      <c r="AA4" t="str">
-        <v/>
-      </c>
-      <c r="AB4" t="str">
-        <v/>
-      </c>
-      <c r="AC4" t="str">
-        <v/>
-      </c>
-      <c r="AD4" t="str">
-        <v/>
-      </c>
-      <c r="AE4" t="str">
-        <v/>
-      </c>
-      <c r="AF4" t="str">
-        <v/>
-      </c>
-      <c r="AG4" t="str">
-        <v/>
-      </c>
-      <c r="AH4" t="str">
-        <v/>
-      </c>
-      <c r="AI4" t="str">
-        <v/>
-      </c>
-      <c r="AJ4" t="str">
-        <v/>
-      </c>
-      <c r="AK4" t="str">
-        <v/>
-      </c>
-      <c r="AL4" t="str">
-        <v/>
-      </c>
-      <c r="AM4" t="str">
-        <v/>
-      </c>
-      <c r="AN4" t="str">
-        <v/>
-      </c>
-      <c r="AO4" t="str">
-        <v/>
-      </c>
-      <c r="AP4" t="str">
-        <v/>
-      </c>
-      <c r="AQ4" t="str">
-        <v/>
-      </c>
-      <c r="AR4" t="str">
-        <v/>
-      </c>
-      <c r="AS4" t="str">
-        <v/>
-      </c>
-      <c r="AT4" t="str">
-        <v/>
-      </c>
-      <c r="AU4" t="str">
-        <v/>
-      </c>
-      <c r="AV4" t="str">
-        <v/>
-      </c>
-      <c r="AW4" t="str">
-        <v/>
-      </c>
-      <c r="AX4" t="str">
-        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AX4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AX2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>